<commit_message>
Add card and bike props
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EEDF8B-999E-46B4-BEF4-276CC6C9C3D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028187E3-E925-48CA-9FB6-1126E6615C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="163">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="162">
   <si>
     <t>Road</t>
   </si>
@@ -68,9 +59,6 @@
     <t>https://tredz.azureedge.net/prodimg/228741-746939_1_Supersize.jpg</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Scott Addict 30 Disc</t>
   </si>
   <si>
@@ -374,15 +362,6 @@
     <t>https://tredz.azureedge.net/prodimg/229742-750824_1_Supersize.jpg</t>
   </si>
   <si>
-    <t>FrameSize</t>
-  </si>
-  <si>
-    <t>FrameMaterial</t>
-  </si>
-  <si>
-    <t>Colour</t>
-  </si>
-  <si>
     <t>Anthracite/Black</t>
   </si>
   <si>
@@ -443,9 +422,6 @@
     <t>12"</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>Haibike</t>
   </si>
   <si>
@@ -458,9 +434,6 @@
     <t>Abalone/Black/Black</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Carbon_Grey</t>
   </si>
   <si>
@@ -513,6 +486,30 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>frameSize</t>
+  </si>
+  <si>
+    <t>frameMaterial</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -556,10 +553,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,1196 +859,1196 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>2020</v>
-      </c>
-      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H2" s="3">
         <v>1208.97</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2">
         <v>2021</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>403.97</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1575.25</v>
+      </c>
+      <c r="I4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>2020</v>
-      </c>
-      <c r="H4">
-        <v>1575.25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>2020</v>
-      </c>
-      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H5" s="3">
         <v>1857.84</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>2020</v>
-      </c>
-      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H6" s="3">
         <v>1447.9</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
         <v>2021</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>1092.76</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>2020</v>
-      </c>
-      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H8" s="3">
         <v>744.26</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>2020</v>
-      </c>
-      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H9" s="3">
         <v>1125.04</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <v>2020</v>
-      </c>
-      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H10" s="3">
         <v>607.82000000000005</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11">
-        <v>2020</v>
-      </c>
-      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H11" s="3">
         <v>1762.82</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2">
         <v>2021</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>577.64</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13">
-        <v>2020</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H13" s="3">
         <v>1283.6300000000001</v>
       </c>
       <c r="I13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2">
         <v>2019</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>1235.53</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>2020</v>
-      </c>
-      <c r="H15">
+      <c r="G15" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H15" s="3">
         <v>1821.8</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2">
         <v>2021</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>1426.79</v>
       </c>
       <c r="I16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17">
-        <v>2020</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H17" s="3">
         <v>379.34</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2">
         <v>2019</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>521.70000000000005</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19">
-        <v>2020</v>
-      </c>
-      <c r="H19">
+      <c r="G19" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H19" s="3">
         <v>1229.22</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20">
-        <v>2020</v>
-      </c>
-      <c r="H20">
+      <c r="G20" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H20" s="3">
         <v>676.88</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>2020</v>
-      </c>
-      <c r="H21">
+      <c r="G21" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H21" s="3">
         <v>364.45</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22">
-        <v>2020</v>
-      </c>
-      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H22" s="3">
         <v>1429.11</v>
       </c>
       <c r="I22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23">
-        <v>2020</v>
-      </c>
-      <c r="H23">
+        <v>6</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H23" s="3">
         <v>1092.3499999999999</v>
       </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24">
-        <v>2020</v>
-      </c>
-      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H24" s="3">
         <v>528.92999999999995</v>
       </c>
       <c r="I24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25">
-        <v>2020</v>
-      </c>
-      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H25" s="3">
         <v>1090.44</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26">
-        <v>2020</v>
-      </c>
-      <c r="H26">
+      <c r="G26" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H26" s="3">
         <v>1849.42</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27">
-        <v>2020</v>
-      </c>
-      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H27" s="3">
         <v>753.61</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28">
-        <v>2020</v>
-      </c>
-      <c r="H28">
+        <v>6</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H28" s="3">
         <v>1573.85</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2">
         <v>2021</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>1801.22</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30">
-        <v>2020</v>
-      </c>
-      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H30" s="3">
         <v>587.66</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31">
-        <v>2020</v>
-      </c>
-      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H31" s="3">
         <v>1684.73</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32">
+        <v>6</v>
+      </c>
+      <c r="G32" s="2">
         <v>2021</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>427.76</v>
       </c>
       <c r="I32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1359.8</v>
+      </c>
+      <c r="I33" t="s">
         <v>93</v>
-      </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33">
-        <v>2021</v>
-      </c>
-      <c r="H33">
-        <v>1359.8</v>
-      </c>
-      <c r="I33" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F34" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34">
+        <v>6</v>
+      </c>
+      <c r="G34" s="2">
         <v>2021</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>819.61</v>
       </c>
       <c r="I34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F35" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35">
-        <v>2020</v>
-      </c>
-      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H35" s="3">
         <v>819.95</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="G36" s="2">
         <v>2019</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="3">
         <v>452.75</v>
       </c>
       <c r="I36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="G37" s="2">
         <v>2021</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="3">
         <v>1107.67</v>
       </c>
       <c r="I37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38">
-        <v>2020</v>
-      </c>
-      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H38" s="3">
         <v>1205.98</v>
       </c>
       <c r="I38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F39" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="G39" s="2">
         <v>2021</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="3">
         <v>1166.06</v>
       </c>
       <c r="I39" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="G40" s="2">
         <v>2022</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="3">
         <v>1653.37</v>
       </c>
       <c r="I40" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F41" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41">
-        <v>2020</v>
-      </c>
-      <c r="H41">
+        <v>6</v>
+      </c>
+      <c r="G41" s="2">
+        <v>2020</v>
+      </c>
+      <c r="H41" s="3">
         <v>1581.64</v>
       </c>
       <c r="I41" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2069,15 +2067,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -2085,7 +2083,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -2093,7 +2091,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2101,7 +2099,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -2109,7 +2107,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2117,7 +2115,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2125,7 +2123,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -2133,7 +2131,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -2141,7 +2139,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -2149,7 +2147,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2157,7 +2155,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -2165,7 +2163,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -2173,7 +2171,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -2181,7 +2179,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -2189,7 +2187,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -2197,7 +2195,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -2205,7 +2203,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -2213,7 +2211,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -2221,7 +2219,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -2229,7 +2227,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -2237,7 +2235,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -2245,7 +2243,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -2253,7 +2251,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -2261,7 +2259,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -2269,7 +2267,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -2277,7 +2275,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2285,7 +2283,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -2293,7 +2291,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -2301,7 +2299,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -2309,7 +2307,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -2317,7 +2315,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -2325,7 +2323,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -2333,7 +2331,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -2341,7 +2339,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B35">
         <v>10</v>
@@ -2349,7 +2347,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -2357,7 +2355,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -2365,7 +2363,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -2373,7 +2371,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -2381,7 +2379,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B40">
         <v>10</v>
@@ -2389,7 +2387,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B41">
         <v>10</v>

</xml_diff>